<commit_message>
cap nhat bieu do
</commit_message>
<xml_diff>
--- a/src/main/resources/DataImports/SanPham.xlsx
+++ b/src/main/resources/DataImports/SanPham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PTUD_APP\Manager_QuanLyHieuSach\src\main\resources\DataImports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BBBE9A-E009-41D1-B49D-B2A35426FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6D7000-3A90-4ED1-9CED-4CB0C8237118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4A98E7E-91B4-4117-82EF-535CA966D02F}"/>
   </bookViews>
@@ -667,7 +667,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -728,22 +728,22 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f ca="1">"SP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A1), "0000")</f>
-        <v>SP202312090001</v>
+        <v>SP202312120001</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="3" t="str">
         <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312090010</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D2" s="3" t="str">
         <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312090019</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>16</v>
+        <v>10.6</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -768,28 +768,28 @@
       </c>
       <c r="L2" s="4">
         <f ca="1">ROUNDUP(K2 * CHOOSE(RANDBETWEEN(1, 4),0.1, 0.2, 0.3,0), 2)</f>
-        <v>0</v>
+        <v>110700</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f t="shared" ref="A3:A62" ca="1" si="0">"SP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A2), "0000")</f>
-        <v>SP202312090002</v>
+        <v>SP202312120002</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:C62" ca="1" si="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312090010</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D62" ca="1" si="2">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312090007</v>
+        <v>NCC202312120001</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>9.6</v>
+        <v>15.5</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -814,35 +814,35 @@
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3:L62" ca="1" si="6">ROUNDUP(K3 * CHOOSE(RANDBETWEEN(1, 4),0.1, 0.2, 0.3,0), 2)</f>
-        <v>102500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090003</v>
+        <v>SP202312120003</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090020</v>
+        <v>NCC202312120020</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E62" ca="1" si="7">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>25.9</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="4"/>
@@ -860,28 +860,28 @@
       </c>
       <c r="L4" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>28700</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090004</v>
+        <v>SP202312120004</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090004</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090022</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>15.8</v>
+        <v>28.5</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -906,35 +906,35 @@
       </c>
       <c r="L5" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>328000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090005</v>
+        <v>SP202312120005</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>6.8</v>
+        <v>23.6</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="4"/>
@@ -958,22 +958,22 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090006</v>
+        <v>SP202312120006</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090003</v>
+        <v>NCC202312120008</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>14.6</v>
+        <v>8.6</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>23</v>
@@ -998,28 +998,28 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>43050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090007</v>
+        <v>SP202312120007</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090002</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>13.3</v>
+        <v>11.2</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>25</v>
@@ -1044,28 +1044,28 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090008</v>
+        <v>SP202312120008</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090005</v>
+        <v>NCC202312120009</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>24.4</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
@@ -1090,28 +1090,28 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>615000</v>
+        <v>922500</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090009</v>
+        <v>SP202312120009</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090005</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090011</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>26.1</v>
+        <v>21.6</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -1136,35 +1136,35 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>41000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090010</v>
+        <v>SP202312120010</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120009</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>20.399999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="4"/>
@@ -1188,22 +1188,22 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090011</v>
+        <v>SP202312120011</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090023</v>
+        <v>NCC202312120008</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>5.8</v>
+        <v>28.6</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
@@ -1234,29 +1234,29 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090012</v>
+        <v>SP202312120012</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090010</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090016</v>
+        <v>NCC202312120010</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9.8000000000000007</v>
+        <v>5.7</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="4"/>
@@ -1274,35 +1274,35 @@
       </c>
       <c r="L13" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>184500</v>
+        <v>123000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090013</v>
+        <v>SP202312120013</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090003</v>
+        <v>NCC202312120017</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>28.6</v>
+        <v>5.3</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="4"/>
@@ -1320,28 +1320,28 @@
       </c>
       <c r="L14" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>24600</v>
+        <v>73800</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090014</v>
+        <v>SP202312120014</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090014</v>
+        <v>NCC202312120023</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>16.2</v>
+        <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>35</v>
@@ -1366,35 +1366,35 @@
       </c>
       <c r="L15" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>143500</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090015</v>
+        <v>SP202312120015</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090002</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090006</v>
+        <v>NCC202312120007</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>19.5</v>
+        <v>9.1</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="4"/>
@@ -1412,35 +1412,35 @@
       </c>
       <c r="L16" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>102500</v>
+        <v>51250</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090016</v>
+        <v>SP202312120016</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090010</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090008</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>24.4</v>
+        <v>8.4</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="4"/>
@@ -1458,28 +1458,28 @@
       </c>
       <c r="L17" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>153750</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090017</v>
+        <v>SP202312120017</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090002</v>
+        <v>NCC202312120001</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>24</v>
+        <v>14.8</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
@@ -1510,29 +1510,29 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090018</v>
+        <v>SP202312120018</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090002</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>17.899999999999999</v>
+        <v>10.4</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="4"/>
@@ -1556,29 +1556,29 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090019</v>
+        <v>SP202312120019</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090022</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>16.3</v>
+        <v>27.5</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="4"/>
@@ -1596,35 +1596,35 @@
       </c>
       <c r="L20" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>110700</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090020</v>
+        <v>SP202312120020</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090010</v>
+        <v>NCC202312120011</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>12.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="4"/>
@@ -1648,22 +1648,22 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090021</v>
+        <v>SP202312120021</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9.8000000000000007</v>
+        <v>10.5</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>43</v>
@@ -1688,28 +1688,28 @@
       </c>
       <c r="L22" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>20500</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090022</v>
+        <v>SP202312120022</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090016</v>
+        <v>NCC202312120008</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>16.8</v>
+        <v>19.5</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>45</v>
@@ -1734,28 +1734,28 @@
       </c>
       <c r="L23" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>10250</v>
+        <v>15375</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090023</v>
+        <v>SP202312120023</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090007</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>22.4</v>
+        <v>26.4</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>21</v>
@@ -1780,28 +1780,28 @@
       </c>
       <c r="L24" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>16400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090024</v>
+        <v>SP202312120024</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090011</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>14.3</v>
+        <v>21.5</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
@@ -1826,35 +1826,35 @@
       </c>
       <c r="L25" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>6150</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090025</v>
+        <v>SP202312120025</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090010</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>15.3</v>
+        <v>15.4</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="4"/>
@@ -1872,28 +1872,28 @@
       </c>
       <c r="L26" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>21525</v>
+        <v>14350</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090026</v>
+        <v>SP202312120026</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090015</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>5.9</v>
+        <v>26.7</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
@@ -1918,35 +1918,35 @@
       </c>
       <c r="L27" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>61500</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090027</v>
+        <v>SP202312120027</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090011</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9.4</v>
+        <v>22.6</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="4"/>
@@ -1970,29 +1970,29 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090028</v>
+        <v>SP202312120028</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090003</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>18.600000000000001</v>
+        <v>25.2</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="4"/>
@@ -2010,28 +2010,28 @@
       </c>
       <c r="L29" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>184500</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090029</v>
+        <v>SP202312120029</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120007</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>19.3</v>
+        <v>11.8</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>54</v>
@@ -2056,28 +2056,28 @@
       </c>
       <c r="L30" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>16400</v>
+        <v>32800</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090030</v>
+        <v>SP202312120030</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090010</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120011</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>10.7</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>25</v>
@@ -2102,35 +2102,35 @@
       </c>
       <c r="L31" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>4100</v>
+        <v>12300</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090031</v>
+        <v>SP202312120031</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>7.5</v>
+        <v>23.6</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="4"/>
@@ -2154,22 +2154,22 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090032</v>
+        <v>SP202312120032</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090004</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>23</v>
+        <v>14.8</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>31</v>
@@ -2194,35 +2194,35 @@
       </c>
       <c r="L33" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>153750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090033</v>
+        <v>SP202312120033</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090010</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120013</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>27.6</v>
+        <v>20</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="4"/>
@@ -2246,29 +2246,29 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090034</v>
+        <v>SP202312120034</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090002</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090016</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>19.2</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="4"/>
@@ -2292,22 +2292,22 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090035</v>
+        <v>SP202312120035</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090005</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090014</v>
+        <v>NCC202312120014</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>18.3</v>
+        <v>16.8</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>23</v>
@@ -2332,35 +2332,35 @@
       </c>
       <c r="L36" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>10250</v>
+        <v>30750</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090036</v>
+        <v>SP202312120036</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C37" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090021</v>
+        <v>NCC202312120007</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>5.8</v>
+        <v>24.2</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="4">
         <f t="shared" si="4"/>
@@ -2378,28 +2378,28 @@
       </c>
       <c r="L37" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>32800</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090037</v>
+        <v>SP202312120037</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C38" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090004</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090011</v>
+        <v>NCC202312120001</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>8.3000000000000007</v>
+        <v>19.7</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
@@ -2424,28 +2424,28 @@
       </c>
       <c r="L38" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>36900</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090038</v>
+        <v>SP202312120038</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9.6999999999999993</v>
+        <v>11.6</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>31</v>
@@ -2470,28 +2470,28 @@
       </c>
       <c r="L39" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>49200</v>
+        <v>73800</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090039</v>
+        <v>SP202312120039</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120022</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>22.7</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>21</v>
@@ -2516,28 +2516,28 @@
       </c>
       <c r="L40" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>61500</v>
+        <v>30750</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090040</v>
+        <v>SP202312120040</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090005</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090014</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>25</v>
@@ -2562,28 +2562,28 @@
       </c>
       <c r="L41" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>123000</v>
+        <v>41000</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090041</v>
+        <v>SP202312120041</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C42" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090010</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>21</v>
+        <v>9.5</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>19</v>
@@ -2608,28 +2608,28 @@
       </c>
       <c r="L42" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>92250</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090042</v>
+        <v>SP202312120042</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C43" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090005</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090015</v>
+        <v>NCC202312120009</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>17.3</v>
+        <v>12.8</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>21</v>
@@ -2654,35 +2654,35 @@
       </c>
       <c r="L43" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>12300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090043</v>
+        <v>SP202312120043</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C44" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120010</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>24.7</v>
+        <v>14</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G44" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="4"/>
@@ -2700,28 +2700,28 @@
       </c>
       <c r="L44" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>8200</v>
+        <v>12300</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090044</v>
+        <v>SP202312120044</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C45" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090009</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>13.1</v>
+        <v>16.3</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>43</v>
@@ -2752,22 +2752,22 @@
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090045</v>
+        <v>SP202312120045</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C46" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090001</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>11.5</v>
+        <v>6</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>21</v>
@@ -2792,28 +2792,28 @@
       </c>
       <c r="L46" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>6150</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090046</v>
+        <v>SP202312120046</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C47" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090017</v>
+        <v>NCC202312120016</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>12.4</v>
+        <v>27.4</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>54</v>
@@ -2844,22 +2844,22 @@
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090047</v>
+        <v>SP202312120047</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C48" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090023</v>
+        <v>NCC202312120013</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>27.5</v>
+        <v>13.5</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>13</v>
@@ -2890,22 +2890,22 @@
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090048</v>
+        <v>SP202312120048</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C49" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090021</v>
+        <v>NCC202312120016</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>18.3</v>
+        <v>10.5</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>25</v>
@@ -2930,28 +2930,28 @@
       </c>
       <c r="L49" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>6150</v>
+        <v>12300</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090049</v>
+        <v>SP202312120049</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C50" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090004</v>
+        <v>NCC202312120022</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>8.3000000000000007</v>
+        <v>23.8</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>21</v>
@@ -2976,28 +2976,28 @@
       </c>
       <c r="L50" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>492000</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090050</v>
+        <v>SP202312120050</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090016</v>
+        <v>NCC202312120006</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>20.399999999999999</v>
+        <v>21.2</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>21</v>
@@ -3022,35 +3022,35 @@
       </c>
       <c r="L51" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>32800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090051</v>
+        <v>SP202312120051</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C52" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>10.199999999999999</v>
+        <v>29</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" s="4">
         <f t="shared" si="4"/>
@@ -3074,29 +3074,29 @@
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090052</v>
+        <v>SP202312120052</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C53" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090002</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090005</v>
+        <v>NCC202312120014</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>14.3</v>
+        <v>25.9</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G53" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" si="4"/>
@@ -3114,35 +3114,35 @@
       </c>
       <c r="L53" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>12300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090053</v>
+        <v>SP202312120053</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090002</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090019</v>
+        <v>NCC202312120013</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>7.6</v>
+        <v>12.5</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G54" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="4"/>
@@ -3160,28 +3160,28 @@
       </c>
       <c r="L54" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>24600</v>
+        <v>16400</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090054</v>
+        <v>SP202312120054</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C55" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090008</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090012</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>6.4</v>
+        <v>13</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>13</v>
@@ -3206,35 +3206,35 @@
       </c>
       <c r="L55" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>49200</v>
+        <v>32800</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090055</v>
+        <v>SP202312120055</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C56" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090017</v>
+        <v>NCC202312120007</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>9.1999999999999993</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G56" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="4"/>
@@ -3252,35 +3252,35 @@
       </c>
       <c r="L56" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>615000</v>
+        <v>922500</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090056</v>
+        <v>SP202312120056</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C57" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090006</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090012</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>13</v>
+        <v>26.1</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>81</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="4"/>
@@ -3298,28 +3298,28 @@
       </c>
       <c r="L57" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>102500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090057</v>
+        <v>SP202312120057</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C58" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090011</v>
+        <v>NCC202312120023</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>23.3</v>
+        <v>27.3</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>21</v>
@@ -3350,22 +3350,22 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090058</v>
+        <v>SP202312120058</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C59" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090004</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090015</v>
+        <v>NCC202312120013</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>11.3</v>
+        <v>20.8</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>25</v>
@@ -3396,22 +3396,22 @@
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090059</v>
+        <v>SP202312120059</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C60" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090003</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090023</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>10.8</v>
+        <v>9</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>21</v>
@@ -3436,28 +3436,28 @@
       </c>
       <c r="L60" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090060</v>
+        <v>SP202312120060</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C61" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090007</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D61" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090013</v>
+        <v>NCC202312120002</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>19.2</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>23</v>
@@ -3488,29 +3488,29 @@
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SP202312090061</v>
+        <v>SP202312120061</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C62" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312090009</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D62" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312090022</v>
+        <v>NCC202312120010</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <v>21.9</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
hoan thanh thong ke sp
</commit_message>
<xml_diff>
--- a/src/main/resources/DataImports/SanPham.xlsx
+++ b/src/main/resources/DataImports/SanPham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PTUD_APP\Manager_QuanLyHieuSach\src\main\resources\DataImports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6D7000-3A90-4ED1-9CED-4CB0C8237118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52F0BA1-C8A6-4BBE-A67F-92C30320BDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4A98E7E-91B4-4117-82EF-535CA966D02F}"/>
   </bookViews>
@@ -368,9 +368,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,7 +408,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -514,7 +514,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -656,7 +656,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB6A4C7-4B50-4675-8CC3-47D0FEE36865}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -735,15 +735,15 @@
       </c>
       <c r="C2" s="3" t="str">
         <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312120006</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D2" s="3" t="str">
         <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312120019</v>
+        <v>NCC202312120001</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>10.6</v>
+        <v>14.5</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -767,8 +767,7 @@
         <v>369000</v>
       </c>
       <c r="L2" s="4">
-        <f ca="1">ROUNDUP(K2 * CHOOSE(RANDBETWEEN(1, 4),0.1, 0.2, 0.3,0), 2)</f>
-        <v>110700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -781,15 +780,15 @@
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:C62" ca="1" si="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312120008</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D62" ca="1" si="2">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312120001</v>
+        <v>NCC202312120023</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>15.5</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -813,7 +812,6 @@
         <v>1025000</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L62" ca="1" si="6">ROUNDUP(K3 * CHOOSE(RANDBETWEEN(1, 4),0.1, 0.2, 0.3,0), 2)</f>
         <v>0</v>
       </c>
     </row>
@@ -827,15 +825,15 @@
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120003</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120020</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E62" ca="1" si="7">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>25</v>
+        <f t="shared" ref="E4:E62" ca="1" si="6">ROUND(RAND()*(30-5)+5, 1)</f>
+        <v>25.8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -859,8 +857,7 @@
         <v>143500</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>28700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -877,18 +874,18 @@
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>28.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>29.5</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="4"/>
@@ -905,8 +902,7 @@
         <v>1640000</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>328000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -923,11 +919,11 @@
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120004</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>23.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
@@ -951,8 +947,7 @@
         <v>615000</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>184500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -965,15 +960,15 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120004</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120008</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>23</v>
@@ -997,7 +992,6 @@
         <v>143500</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1011,15 +1005,15 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120005</v>
+        <v>NCC202312120017</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>11.2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>25</v>
@@ -1043,7 +1037,6 @@
         <v>102500</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1057,15 +1050,15 @@
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120006</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120009</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>22.1</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
@@ -1089,8 +1082,7 @@
         <v>3075000</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>922500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1107,18 +1099,18 @@
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120012</v>
+        <v>NCC202312120017</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>21.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>28.4</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="4"/>
@@ -1135,7 +1127,6 @@
         <v>410000</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1149,22 +1140,22 @@
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120009</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.6999999999999993</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>13.9</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="4"/>
@@ -1181,8 +1172,7 @@
         <v>246000</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>49200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1195,15 +1185,15 @@
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>NCC202312120008</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>28.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>11.9</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
@@ -1227,8 +1217,7 @@
         <v>184500</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>36900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1241,22 +1230,22 @@
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120005</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120010</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>5.7</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="4"/>
@@ -1273,8 +1262,7 @@
         <v>615000</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>123000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1291,11 +1279,11 @@
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120017</v>
+        <v>NCC202312120022</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>5.3</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -1319,8 +1307,7 @@
         <v>246000</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>73800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1333,22 +1320,22 @@
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120023</v>
+        <v>NCC202312120016</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="4"/>
@@ -1365,8 +1352,7 @@
         <v>717500</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>143500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1379,22 +1365,22 @@
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120007</v>
+        <v>NCC202312120013</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>9.1</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="4"/>
@@ -1411,8 +1397,7 @@
         <v>512500</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>51250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,15 +1410,15 @@
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120012</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>11.9</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
@@ -1457,8 +1442,7 @@
         <v>512500</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>153750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,22 +1455,22 @@
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120001</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>14.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>9.6</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="4"/>
@@ -1503,7 +1487,6 @@
         <v>164000</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1517,22 +1500,22 @@
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120006</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120019</v>
+        <v>NCC202312120008</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.5</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="4"/>
@@ -1549,8 +1532,7 @@
         <v>410000</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>41000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1563,22 +1545,22 @@
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120019</v>
+        <v>NCC202312120014</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>27.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.2</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="4"/>
@@ -1595,8 +1577,7 @@
         <v>369000</v>
       </c>
       <c r="L20" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>110700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1609,22 +1590,22 @@
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120011</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>5.0999999999999996</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>23.5</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="4"/>
@@ -1641,7 +1622,6 @@
         <v>246000</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1659,11 +1639,11 @@
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120012</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>23.8</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>43</v>
@@ -1687,8 +1667,7 @@
         <v>102500</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>20500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1701,22 +1680,22 @@
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120008</v>
+        <v>NCC202312120016</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>19.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>13.4</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="4"/>
@@ -1733,8 +1712,7 @@
         <v>51250</v>
       </c>
       <c r="L23" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>15375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1747,15 +1725,15 @@
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120004</v>
+        <v>NCC202312120010</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>26.4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7.8</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>21</v>
@@ -1779,7 +1757,6 @@
         <v>164000</v>
       </c>
       <c r="L24" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1793,15 +1770,15 @@
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120003</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>21.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18.899999999999999</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
@@ -1825,8 +1802,7 @@
         <v>61500</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>6150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1839,15 +1815,15 @@
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120019</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>15.4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>13.8</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>19</v>
@@ -1871,8 +1847,7 @@
         <v>71750</v>
       </c>
       <c r="L26" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>14350</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1885,15 +1860,15 @@
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120015</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>26.7</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>22.6</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
@@ -1917,8 +1892,7 @@
         <v>307500</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>61500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1931,15 +1905,15 @@
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120023</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>22.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>28.7</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>51</v>
@@ -1963,8 +1937,7 @@
         <v>143500</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>43050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1977,22 +1950,22 @@
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120004</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120003</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>25.2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>11.5</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="4"/>
@@ -2009,8 +1982,7 @@
         <v>615000</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>184500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2023,22 +1995,22 @@
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120007</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>11.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>26.2</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="4"/>
@@ -2055,8 +2027,7 @@
         <v>164000</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>32800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2069,15 +2040,15 @@
       </c>
       <c r="C31" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120003</v>
+        <v>LSP202312120004</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120011</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>17.399999999999999</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>11.6</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>25</v>
@@ -2101,8 +2072,7 @@
         <v>41000</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>12300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2115,22 +2085,22 @@
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120017</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>23.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.6</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="4"/>
@@ -2147,8 +2117,7 @@
         <v>61500</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>18450</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2165,11 +2134,11 @@
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120012</v>
+        <v>NCC202312120006</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>14.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>13.7</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>31</v>
@@ -2193,7 +2162,6 @@
         <v>512500</v>
       </c>
       <c r="L33" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2207,22 +2175,22 @@
       </c>
       <c r="C34" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120013</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18.899999999999999</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="4"/>
@@ -2239,8 +2207,7 @@
         <v>143500</v>
       </c>
       <c r="L34" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>43050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2257,18 +2224,18 @@
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120012</v>
+        <v>NCC202312120007</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>19.2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>29.1</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="4"/>
@@ -2285,8 +2252,7 @@
         <v>246000</v>
       </c>
       <c r="L35" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>49200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,22 +2265,22 @@
       </c>
       <c r="C36" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120005</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120014</v>
+        <v>NCC202312120020</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>16.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>28.3</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="4"/>
@@ -2331,8 +2297,7 @@
         <v>102500</v>
       </c>
       <c r="L36" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2345,22 +2310,22 @@
       </c>
       <c r="C37" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120005</v>
+        <v>LSP202312120002</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120007</v>
+        <v>NCC202312120003</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>24.2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>24.4</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="4">
         <f t="shared" si="4"/>
@@ -2377,8 +2342,7 @@
         <v>164000</v>
       </c>
       <c r="L37" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>32800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2391,22 +2355,22 @@
       </c>
       <c r="C38" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120001</v>
+        <v>NCC202312120015</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>19.7</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8.5</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="4">
         <f t="shared" si="4"/>
@@ -2423,8 +2387,7 @@
         <v>123000</v>
       </c>
       <c r="L38" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>24600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2437,22 +2400,22 @@
       </c>
       <c r="C39" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120006</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120005</v>
+        <v>NCC202312120020</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>11.6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18.5</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="4">
         <f t="shared" si="4"/>
@@ -2469,8 +2432,7 @@
         <v>246000</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>73800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2487,11 +2449,11 @@
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120022</v>
+        <v>NCC202312120010</v>
       </c>
       <c r="E40" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>19.600000000000001</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>26</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>21</v>
@@ -2515,8 +2477,7 @@
         <v>307500</v>
       </c>
       <c r="L40" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>30750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2533,11 +2494,11 @@
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E41" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>25.9</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>25</v>
@@ -2561,8 +2522,7 @@
         <v>410000</v>
       </c>
       <c r="L41" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>41000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2575,15 +2535,15 @@
       </c>
       <c r="C42" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120006</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120019</v>
+        <v>NCC202312120005</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>9.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>21.4</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>19</v>
@@ -2607,8 +2567,7 @@
         <v>307500</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>92250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2625,11 +2584,11 @@
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120009</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>12.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>29.4</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>21</v>
@@ -2653,7 +2612,6 @@
         <v>123000</v>
       </c>
       <c r="L43" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2667,15 +2625,15 @@
       </c>
       <c r="C44" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120010</v>
+        <v>NCC202312120018</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7.5</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>25</v>
@@ -2699,8 +2657,7 @@
         <v>41000</v>
       </c>
       <c r="L44" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>12300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2713,15 +2670,15 @@
       </c>
       <c r="C45" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120015</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>16.3</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>27.9</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>43</v>
@@ -2745,8 +2702,7 @@
         <v>246000</v>
       </c>
       <c r="L45" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>24600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2759,15 +2715,15 @@
       </c>
       <c r="C46" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120005</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.8</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>21</v>
@@ -2791,8 +2747,7 @@
         <v>61500</v>
       </c>
       <c r="L46" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>6150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2805,15 +2760,15 @@
       </c>
       <c r="C47" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120016</v>
+        <v>NCC202312120008</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>27.4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>26.4</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>54</v>
@@ -2837,8 +2792,7 @@
         <v>82000</v>
       </c>
       <c r="L47" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>8200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2851,15 +2805,15 @@
       </c>
       <c r="C48" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120005</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120013</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>13.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>25.8</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>13</v>
@@ -2883,8 +2837,7 @@
         <v>102500</v>
       </c>
       <c r="L48" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>10250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2897,15 +2850,15 @@
       </c>
       <c r="C49" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120007</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120016</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>28.5</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>25</v>
@@ -2929,8 +2882,7 @@
         <v>61500</v>
       </c>
       <c r="L49" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>12300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2947,18 +2899,18 @@
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120022</v>
+        <v>NCC202312120021</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>23.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7.7</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" s="4">
         <f t="shared" si="4"/>
@@ -2975,8 +2927,7 @@
         <v>1640000</v>
       </c>
       <c r="L50" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>492000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2989,15 +2940,15 @@
       </c>
       <c r="C51" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120006</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>21.2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>16.7</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>21</v>
@@ -3021,7 +2972,6 @@
         <v>164000</v>
       </c>
       <c r="L51" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3035,22 +2985,22 @@
       </c>
       <c r="C52" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120014</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8.4</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="4">
         <f t="shared" si="4"/>
@@ -3067,8 +3017,7 @@
         <v>246000</v>
       </c>
       <c r="L52" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>24600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3081,22 +3030,22 @@
       </c>
       <c r="C53" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120005</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120014</v>
+        <v>NCC202312120004</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>25.9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>24.5</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G53" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" si="4"/>
@@ -3113,7 +3062,6 @@
         <v>61500</v>
       </c>
       <c r="L53" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3127,22 +3075,22 @@
       </c>
       <c r="C54" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120002</v>
+        <v>LSP202312120005</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120013</v>
+        <v>NCC202312120019</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>12.5</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>27.8</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G54" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="4"/>
@@ -3159,8 +3107,7 @@
         <v>82000</v>
       </c>
       <c r="L54" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>16400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3173,15 +3120,15 @@
       </c>
       <c r="C55" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120004</v>
+        <v>LSP202312120007</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120015</v>
+        <v>NCC202312120009</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>13</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8.9</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>13</v>
@@ -3205,8 +3152,7 @@
         <v>164000</v>
       </c>
       <c r="L55" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>32800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3219,22 +3165,22 @@
       </c>
       <c r="C56" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120010</v>
+        <v>LSP202312120003</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120007</v>
+        <v>NCC202312120023</v>
       </c>
       <c r="E56" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>18.100000000000001</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18.7</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G56" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="4"/>
@@ -3251,8 +3197,7 @@
         <v>3075000</v>
       </c>
       <c r="L56" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>922500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3265,22 +3210,22 @@
       </c>
       <c r="C57" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120010</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120021</v>
+        <v>NCC202312120018</v>
       </c>
       <c r="E57" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>26.1</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18.7</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>81</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="4"/>
@@ -3297,7 +3242,6 @@
         <v>512500</v>
       </c>
       <c r="L57" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3311,15 +3255,15 @@
       </c>
       <c r="C58" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120009</v>
+        <v>LSP202312120008</v>
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120023</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E58" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>27.3</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>17.5</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>21</v>
@@ -3343,8 +3287,7 @@
         <v>1435000</v>
       </c>
       <c r="L58" s="4">
-        <f t="shared" ca="1" si="6"/>
-        <v>143500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3357,15 +3300,15 @@
       </c>
       <c r="C59" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120003</v>
+        <v>LSP202312120006</v>
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120013</v>
+        <v>NCC202312120018</v>
       </c>
       <c r="E59" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.8</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>24.7</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>25</v>
@@ -3389,7 +3332,6 @@
         <v>615000</v>
       </c>
       <c r="L59" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3403,22 +3345,22 @@
       </c>
       <c r="C60" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120005</v>
+        <v>NCC202312120012</v>
       </c>
       <c r="E60" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>15.9</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G60" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="4"/>
@@ -3435,7 +3377,6 @@
         <v>307500</v>
       </c>
       <c r="L60" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3453,11 +3394,11 @@
       </c>
       <c r="D61" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NCC202312120002</v>
+        <v>NCC202312120011</v>
       </c>
       <c r="E61" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.3000000000000007</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>23.8</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>23</v>
@@ -3481,7 +3422,6 @@
         <v>1230000</v>
       </c>
       <c r="L61" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3495,15 +3435,15 @@
       </c>
       <c r="C62" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LSP202312120008</v>
+        <v>LSP202312120009</v>
       </c>
       <c r="D62" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>NCC202312120010</v>
       </c>
       <c r="E62" s="3">
-        <f t="shared" ca="1" si="7"/>
-        <v>21.9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>19.600000000000001</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
@@ -3527,7 +3467,6 @@
         <v>410000</v>
       </c>
       <c r="L62" s="4">
-        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cap nhat exxcel san pham
</commit_message>
<xml_diff>
--- a/src/main/resources/DataImports/SanPham.xlsx
+++ b/src/main/resources/DataImports/SanPham.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PTUD_APP\Manager_QuanLyHieuSach\src\main\resources\DataImports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC01EB-A9A3-4D83-B3D3-0ED0ED3ECC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C983C-8382-4EE8-B826-58B0C8278A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4A98E7E-91B4-4117-82EF-535CA966D02F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trang_tính3" sheetId="3" r:id="rId1"/>
+    <sheet name="Trang_tính2" sheetId="2" r:id="rId2"/>
+    <sheet name="Trang_tính1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Trang_tính1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Trang_tính1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Trang_tính3!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="150">
   <si>
     <t>idSanPham</t>
   </si>
@@ -297,6 +300,198 @@
   </si>
   <si>
     <t>Gương trang điểm LED</t>
+  </si>
+  <si>
+    <t>idLoaiSanPham</t>
+  </si>
+  <si>
+    <t>tenLoaiSanPham</t>
+  </si>
+  <si>
+    <t>Đồ chơi</t>
+  </si>
+  <si>
+    <t>Sách</t>
+  </si>
+  <si>
+    <t>Phim và album</t>
+  </si>
+  <si>
+    <t>Trò chơi giáo dục</t>
+  </si>
+  <si>
+    <t>Bản đồ</t>
+  </si>
+  <si>
+    <t>Dấu trang</t>
+  </si>
+  <si>
+    <t>Văn phòng phẩm</t>
+  </si>
+  <si>
+    <t>Bút mực trang trí</t>
+  </si>
+  <si>
+    <t>Thiệp chúc mừng và thiệp ghi chú trống</t>
+  </si>
+  <si>
+    <t>Trò chơi bảng</t>
+  </si>
+  <si>
+    <t>idNhaCungCap</t>
+  </si>
+  <si>
+    <t>tenNhaCungCap</t>
+  </si>
+  <si>
+    <t>diaChi</t>
+  </si>
+  <si>
+    <t>soDienThoai</t>
+  </si>
+  <si>
+    <t>Công ty Điện tử Minh Châu</t>
+  </si>
+  <si>
+    <t>Công ty Thời trang Áo Đẹp</t>
+  </si>
+  <si>
+    <t>Công ty Đồ gia dụng Hạnh Phúc</t>
+  </si>
+  <si>
+    <t>Công ty Mỹ phẩm Tâm Anh</t>
+  </si>
+  <si>
+    <t>Công ty Quà lưu niệm Vui Vẻ</t>
+  </si>
+  <si>
+    <t>Công ty Sách Hữu Nghị</t>
+  </si>
+  <si>
+    <t>Công ty Đồ chơi Trí Tuệ</t>
+  </si>
+  <si>
+    <t>Công ty Nước hoa Thanh Xuân</t>
+  </si>
+  <si>
+    <t>Công ty Đồ điện gia dụng Tiến Đạt</t>
+  </si>
+  <si>
+    <t>Công ty Phụ kiện Thời trang Sang Trọng</t>
+  </si>
+  <si>
+    <t>Công ty Sách Văn Học Việt Nam</t>
+  </si>
+  <si>
+    <t>Công ty Sách Giáo Khoa Thành Phố</t>
+  </si>
+  <si>
+    <t>Công ty Văn Phòng Phẩm Thái Bình</t>
+  </si>
+  <si>
+    <t>Công ty Đồ Dùng Học Tập Huy Hoàng</t>
+  </si>
+  <si>
+    <t>Công ty Sách Ngoại Văn Anh Văn</t>
+  </si>
+  <si>
+    <t>Công ty Quà Tặng Văn Hóa Việt</t>
+  </si>
+  <si>
+    <t>Công ty Sách Khoa Học Kỹ Thuật</t>
+  </si>
+  <si>
+    <t>Công ty Đồ Chơi Giáo Dục Thông Minh</t>
+  </si>
+  <si>
+    <t>890 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>891 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>892 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>893 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>894 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>895 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>896 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>897 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>898 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>899 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>900 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>901 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>902 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>903 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>904 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>905 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>906 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>907 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>908 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>909 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>910 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>911 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>912 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>913 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>914 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>915 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>916 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>917 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>918 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>hoang</t>
   </si>
 </sst>
 </file>
@@ -306,10 +501,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;₫&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -336,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -350,6 +552,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -663,11 +867,682 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E5C01E-DF7C-47B1-A3AD-5B43A2BED607}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="str">
+        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
+        <v>NCC202312130019</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="str">
+        <f t="shared" ref="A3:D23" ca="1" si="0">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
+        <v>NCC202312130011</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130014</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130008</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130007</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130002</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130021</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130006</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130009</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130017</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130007</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130023</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130011</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130020</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130013</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130021</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130013</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130009</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130011</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130005</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130022</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130001</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="str">
+        <f t="shared" ref="A24:A30" ca="1" si="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
+        <v>NCC202312130014</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130011</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130014</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130022</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130001</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130014</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D26" xr:uid="{35E5C01E-DF7C-47B1-A3AD-5B43A2BED607}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8B4145-E7A7-4BF3-B67B-1D4E4FEF9CC8}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
+        <v>LSP202312130007</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A20" ca="1" si="0">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
+        <v>LSP202312130007</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130006</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130009</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130009</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130007</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130008</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130007</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130009</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130005</v>
+      </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130002</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130004</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130006</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130009</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LSP202312130010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB6A4C7-4B50-4675-8CC3-47D0FEE36865}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -735,15 +1610,15 @@
       </c>
       <c r="C2" s="3" t="str">
         <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130010</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D2" s="3" t="str">
         <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130006</v>
+        <v>NCC202312130001</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>22.8</v>
+        <v>25.5</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -779,26 +1654,26 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:C62" ca="1" si="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130005</v>
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
+        <v>LSP202312130010</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D62" ca="1" si="2">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130017</v>
+        <f t="shared" ref="D3:D62" ca="1" si="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
+        <v>NCC202312130007</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>9.6</v>
+        <v>15.5</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G62" ca="1" si="3">IF(RAND() &lt;= 0.8, 1, 0)</f>
+        <f t="shared" ref="G3:G62" ca="1" si="2">IF(RAND() &lt;= 0.8, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H62" si="4">I3*0.5</f>
+        <f t="shared" ref="H3:H62" si="3">I3*0.5</f>
         <v>250000</v>
       </c>
       <c r="I3" s="4">
@@ -808,7 +1683,7 @@
         <v>25</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K62" si="5">I3+(I3*0.55)+H3</f>
+        <f t="shared" ref="K3:K62" si="4">I3+(I3*0.55)+H3</f>
         <v>1025000</v>
       </c>
       <c r="L3" s="4">
@@ -824,26 +1699,26 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
         <v>LSP202312130004</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130019</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130023</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E62" ca="1" si="6">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>20.3</v>
+        <f t="shared" ref="E4:E62" ca="1" si="5">ROUND(RAND()*(30-5)+5, 1)</f>
+        <v>14.3</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="I4" s="4">
@@ -853,7 +1728,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>143500</v>
       </c>
       <c r="L4" s="4">
@@ -869,26 +1744,26 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130007</v>
+        <f t="shared" ref="C5:C62" ca="1" si="6">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
+        <v>LSP202312130006</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>5.5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>27.1</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>400000</v>
       </c>
       <c r="I5" s="4">
@@ -898,7 +1773,7 @@
         <v>40</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1640000</v>
       </c>
       <c r="L5" s="4">
@@ -914,26 +1789,26 @@
         <v>20</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130007</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130019</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130016</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>17.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>150000</v>
       </c>
       <c r="I6" s="4">
@@ -943,7 +1818,7 @@
         <v>30</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>615000</v>
       </c>
       <c r="L6" s="4">
@@ -959,26 +1834,26 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130009</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130012</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130017</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>22.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>12.5</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="I7" s="4">
@@ -988,7 +1863,7 @@
         <v>60</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>143500</v>
       </c>
       <c r="L7" s="4">
@@ -1004,26 +1879,26 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D8" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130014</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130009</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11.2</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25000</v>
       </c>
       <c r="I8" s="4">
@@ -1033,7 +1908,7 @@
         <v>80</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>102500</v>
       </c>
       <c r="L8" s="4">
@@ -1049,26 +1924,26 @@
         <v>26</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130009</v>
       </c>
       <c r="D9" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130011</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130010</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>16.600000000000001</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>7.7</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>750000</v>
       </c>
       <c r="I9" s="4">
@@ -1078,7 +1953,7 @@
         <v>15</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3075000</v>
       </c>
       <c r="L9" s="4">
@@ -1094,26 +1969,26 @@
         <v>27</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130008</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130022</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23.1</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100000</v>
       </c>
       <c r="I10" s="4">
@@ -1123,7 +1998,7 @@
         <v>70</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>410000</v>
       </c>
       <c r="L10" s="4">
@@ -1139,26 +2014,26 @@
         <v>29</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130007</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130015</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130020</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>25.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>21.1</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I11" s="4">
@@ -1168,7 +2043,7 @@
         <v>90</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L11" s="4">
@@ -1184,26 +2059,26 @@
         <v>30</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130013</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130002</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.2</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45000</v>
       </c>
       <c r="I12" s="4">
@@ -1213,7 +2088,7 @@
         <v>120</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>184500</v>
       </c>
       <c r="L12" s="4">
@@ -1229,26 +2104,26 @@
         <v>32</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130007</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130021</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>24.9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>15.5</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>150000</v>
       </c>
       <c r="I13" s="4">
@@ -1258,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>615000</v>
       </c>
       <c r="L13" s="4">
@@ -1274,26 +2149,26 @@
         <v>33</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130005</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130015</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130023</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>25.3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22.8</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I14" s="4">
@@ -1303,7 +2178,7 @@
         <v>65</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L14" s="4">
@@ -1319,26 +2194,26 @@
         <v>34</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130006</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130013</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8.1999999999999993</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>17.2</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>175000</v>
       </c>
       <c r="I15" s="4">
@@ -1348,7 +2223,7 @@
         <v>20</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>717500</v>
       </c>
       <c r="L15" s="4">
@@ -1364,26 +2239,26 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130008</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130013</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130021</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>9.1999999999999993</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.8</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>125000</v>
       </c>
       <c r="I16" s="4">
@@ -1393,7 +2268,7 @@
         <v>55</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>512500</v>
       </c>
       <c r="L16" s="4">
@@ -1409,26 +2284,26 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130006</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130007</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130001</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>6.5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>10.9</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>125000</v>
       </c>
       <c r="I17" s="4">
@@ -1438,7 +2313,7 @@
         <v>10</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>512500</v>
       </c>
       <c r="L17" s="4">
@@ -1454,26 +2329,26 @@
         <v>38</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130008</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130017</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130005</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>24.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29.2</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I18" s="4">
@@ -1483,7 +2358,7 @@
         <v>85</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L18" s="4">
@@ -1499,26 +2374,26 @@
         <v>39</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130018</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130001</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>19.8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>10.5</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100000</v>
       </c>
       <c r="I19" s="4">
@@ -1528,7 +2403,7 @@
         <v>40</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>410000</v>
       </c>
       <c r="L19" s="4">
@@ -1544,26 +2419,26 @@
         <v>40</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130009</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D20" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130007</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>21.7</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>13.5</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>90000</v>
       </c>
       <c r="I20" s="4">
@@ -1573,7 +2448,7 @@
         <v>30</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>369000</v>
       </c>
       <c r="L20" s="4">
@@ -1589,26 +2464,26 @@
         <v>41</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130002</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130010</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130012</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>16.899999999999999</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>20.2</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I21" s="4">
@@ -1618,7 +2493,7 @@
         <v>65</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L21" s="4">
@@ -1634,26 +2509,26 @@
         <v>42</v>
       </c>
       <c r="C22" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130005</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130002</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.1</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25000</v>
       </c>
       <c r="I22" s="4">
@@ -1663,7 +2538,7 @@
         <v>95</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>102500</v>
       </c>
       <c r="L22" s="4">
@@ -1679,26 +2554,26 @@
         <v>44</v>
       </c>
       <c r="C23" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130006</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130014</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>5.3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12500</v>
       </c>
       <c r="I23" s="4">
@@ -1708,7 +2583,7 @@
         <v>110</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>51250</v>
       </c>
       <c r="L23" s="4">
@@ -1724,26 +2599,26 @@
         <v>46</v>
       </c>
       <c r="C24" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130003</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>14.9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.9</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I24" s="4">
@@ -1753,7 +2628,7 @@
         <v>50</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L24" s="4">
@@ -1769,26 +2644,26 @@
         <v>47</v>
       </c>
       <c r="C25" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130009</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130018</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130019</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>27.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>19.8</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="I25" s="4">
@@ -1798,7 +2673,7 @@
         <v>70</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61500</v>
       </c>
       <c r="L25" s="4">
@@ -1814,26 +2689,26 @@
         <v>48</v>
       </c>
       <c r="C26" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130009</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130020</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130023</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>11.3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18.899999999999999</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17500</v>
       </c>
       <c r="I26" s="4">
@@ -1843,7 +2718,7 @@
         <v>80</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>71750</v>
       </c>
       <c r="L26" s="4">
@@ -1859,26 +2734,26 @@
         <v>49</v>
       </c>
       <c r="C27" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130008</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130017</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130004</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>28.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>20.9</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>75000</v>
       </c>
       <c r="I27" s="4">
@@ -1888,7 +2763,7 @@
         <v>25</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>307500</v>
       </c>
       <c r="L27" s="4">
@@ -1904,26 +2779,26 @@
         <v>50</v>
       </c>
       <c r="C28" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130017</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>14.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.3</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="I28" s="4">
@@ -1933,7 +2808,7 @@
         <v>35</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>143500</v>
       </c>
       <c r="L28" s="4">
@@ -1949,26 +2824,26 @@
         <v>52</v>
       </c>
       <c r="C29" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130017</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130021</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>14.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>16</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>150000</v>
       </c>
       <c r="I29" s="4">
@@ -1978,7 +2853,7 @@
         <v>45</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>615000</v>
       </c>
       <c r="L29" s="4">
@@ -1994,26 +2869,26 @@
         <v>53</v>
       </c>
       <c r="C30" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130005</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130014</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>22.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>17.3</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I30" s="4">
@@ -2023,7 +2898,7 @@
         <v>55</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L30" s="4">
@@ -2039,26 +2914,26 @@
         <v>55</v>
       </c>
       <c r="C31" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130015</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130004</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>15.3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>21.6</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10000</v>
       </c>
       <c r="I31" s="4">
@@ -2068,7 +2943,7 @@
         <v>65</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>41000</v>
       </c>
       <c r="L31" s="4">
@@ -2084,26 +2959,26 @@
         <v>56</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130009</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130002</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130022</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>19.8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>24.2</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="I32" s="4">
@@ -2113,7 +2988,7 @@
         <v>80</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61500</v>
       </c>
       <c r="L32" s="4">
@@ -2129,26 +3004,26 @@
         <v>57</v>
       </c>
       <c r="C33" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130007</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>19.600000000000001</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11.5</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>125000</v>
       </c>
       <c r="I33" s="4">
@@ -2158,7 +3033,7 @@
         <v>40</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>512500</v>
       </c>
       <c r="L33" s="4">
@@ -2174,26 +3049,26 @@
         <v>58</v>
       </c>
       <c r="C34" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130015</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>21.5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6.9</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="I34" s="4">
@@ -2203,7 +3078,7 @@
         <v>55</v>
       </c>
       <c r="K34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>143500</v>
       </c>
       <c r="L34" s="4">
@@ -2219,26 +3094,26 @@
         <v>59</v>
       </c>
       <c r="C35" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130002</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130011</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130004</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>12.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23.9</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I35" s="4">
@@ -2248,7 +3123,7 @@
         <v>70</v>
       </c>
       <c r="K35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L35" s="4">
@@ -2264,26 +3139,26 @@
         <v>60</v>
       </c>
       <c r="C36" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130009</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130020</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130012</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25000</v>
       </c>
       <c r="I36" s="4">
@@ -2293,7 +3168,7 @@
         <v>90</v>
       </c>
       <c r="K36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>102500</v>
       </c>
       <c r="L36" s="4">
@@ -2309,26 +3184,26 @@
         <v>61</v>
       </c>
       <c r="C37" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130009</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130021</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130012</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8.6</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>7.7</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I37" s="4">
@@ -2338,7 +3213,7 @@
         <v>30</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L37" s="4">
@@ -2354,26 +3229,26 @@
         <v>62</v>
       </c>
       <c r="C38" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130007</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130020</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130014</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>22.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30000</v>
       </c>
       <c r="I38" s="4">
@@ -2383,7 +3258,7 @@
         <v>50</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>123000</v>
       </c>
       <c r="L38" s="4">
@@ -2399,26 +3274,26 @@
         <v>63</v>
       </c>
       <c r="C39" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130009</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130020</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130015</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>7.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>19.600000000000001</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I39" s="4">
@@ -2428,7 +3303,7 @@
         <v>35</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L39" s="4">
@@ -2444,26 +3319,26 @@
         <v>64</v>
       </c>
       <c r="C40" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130004</v>
       </c>
       <c r="E40" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.6</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>75000</v>
       </c>
       <c r="I40" s="4">
@@ -2473,7 +3348,7 @@
         <v>60</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>307500</v>
       </c>
       <c r="L40" s="4">
@@ -2489,26 +3364,26 @@
         <v>65</v>
       </c>
       <c r="C41" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="6"/>
         <v>LSP202312130005</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E41" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>15.8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6.1</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100000</v>
       </c>
       <c r="I41" s="4">
@@ -2518,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>410000</v>
       </c>
       <c r="L41" s="4">
@@ -2534,26 +3409,26 @@
         <v>66</v>
       </c>
       <c r="C42" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130007</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130016</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130004</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>75000</v>
       </c>
       <c r="I42" s="4">
@@ -2563,7 +3438,7 @@
         <v>75</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>307500</v>
       </c>
       <c r="L42" s="4">
@@ -2579,26 +3454,26 @@
         <v>67</v>
       </c>
       <c r="C43" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130022</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130019</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>10.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>13.1</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30000</v>
       </c>
       <c r="I43" s="4">
@@ -2608,7 +3483,7 @@
         <v>85</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>123000</v>
       </c>
       <c r="L43" s="4">
@@ -2624,26 +3499,26 @@
         <v>68</v>
       </c>
       <c r="C44" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130016</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18.7</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10000</v>
       </c>
       <c r="I44" s="4">
@@ -2653,7 +3528,7 @@
         <v>100</v>
       </c>
       <c r="K44" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>41000</v>
       </c>
       <c r="L44" s="4">
@@ -2669,26 +3544,26 @@
         <v>69</v>
       </c>
       <c r="C45" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130019</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130010</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>27.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>27.8</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I45" s="4">
@@ -2698,7 +3573,7 @@
         <v>55</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L45" s="4">
@@ -2714,26 +3589,26 @@
         <v>70</v>
       </c>
       <c r="C46" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130015</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130014</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>13.5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>26.6</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="I46" s="4">
@@ -2743,7 +3618,7 @@
         <v>65</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61500</v>
       </c>
       <c r="L46" s="4">
@@ -2759,26 +3634,26 @@
         <v>71</v>
       </c>
       <c r="C47" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130020</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130002</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>23.8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>27.2</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H47" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20000</v>
       </c>
       <c r="I47" s="4">
@@ -2788,7 +3663,7 @@
         <v>80</v>
       </c>
       <c r="K47" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>82000</v>
       </c>
       <c r="L47" s="4">
@@ -2804,26 +3679,26 @@
         <v>72</v>
       </c>
       <c r="C48" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130019</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11.8</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25000</v>
       </c>
       <c r="I48" s="4">
@@ -2833,7 +3708,7 @@
         <v>95</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>102500</v>
       </c>
       <c r="L48" s="4">
@@ -2849,26 +3724,26 @@
         <v>73</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130005</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>20</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="I49" s="4">
@@ -2878,7 +3753,7 @@
         <v>110</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61500</v>
       </c>
       <c r="L49" s="4">
@@ -2894,26 +3769,26 @@
         <v>74</v>
       </c>
       <c r="C50" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>NCC202312130011</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>8.3000000000000007</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.8</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>400000</v>
       </c>
       <c r="I50" s="4">
@@ -2923,7 +3798,7 @@
         <v>40</v>
       </c>
       <c r="K50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1640000</v>
       </c>
       <c r="L50" s="4">
@@ -2939,26 +3814,26 @@
         <v>75</v>
       </c>
       <c r="C51" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130002</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D51" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130022</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25.9</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I51" s="4">
@@ -2968,7 +3843,7 @@
         <v>70</v>
       </c>
       <c r="K51" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L51" s="4">
@@ -2984,26 +3859,26 @@
         <v>76</v>
       </c>
       <c r="C52" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130007</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130011</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>5.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11.3</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H52" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="I52" s="4">
@@ -3013,7 +3888,7 @@
         <v>70</v>
       </c>
       <c r="K52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>246000</v>
       </c>
       <c r="L52" s="4">
@@ -3029,26 +3904,26 @@
         <v>77</v>
       </c>
       <c r="C53" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D53" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130007</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>23.7</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>21.9</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H53" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="I53" s="4">
@@ -3058,7 +3933,7 @@
         <v>12</v>
       </c>
       <c r="K53" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61500</v>
       </c>
       <c r="L53" s="4">
@@ -3074,26 +3949,26 @@
         <v>78</v>
       </c>
       <c r="C54" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130005</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130019</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E54" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>23.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H54" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20000</v>
       </c>
       <c r="I54" s="4">
@@ -3103,7 +3978,7 @@
         <v>18</v>
       </c>
       <c r="K54" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>82000</v>
       </c>
       <c r="L54" s="4">
@@ -3119,26 +3994,26 @@
         <v>79</v>
       </c>
       <c r="C55" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D55" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130020</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29.1</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H55" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="I55" s="4">
@@ -3148,7 +4023,7 @@
         <v>40</v>
       </c>
       <c r="K55" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164000</v>
       </c>
       <c r="L55" s="4">
@@ -3164,26 +4039,26 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130005</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130004</v>
       </c>
       <c r="D56" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130006</v>
       </c>
       <c r="E56" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>22.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H56" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>750000</v>
       </c>
       <c r="I56" s="4">
@@ -3193,7 +4068,7 @@
         <v>25</v>
       </c>
       <c r="K56" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3075000</v>
       </c>
       <c r="L56" s="4">
@@ -3209,26 +4084,26 @@
         <v>52</v>
       </c>
       <c r="C57" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130008</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130002</v>
       </c>
       <c r="D57" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130019</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130013</v>
       </c>
       <c r="E57" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>27.9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>81</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H57" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>125000</v>
       </c>
       <c r="I57" s="4">
@@ -3238,7 +4113,7 @@
         <v>15</v>
       </c>
       <c r="K57" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>512500</v>
       </c>
       <c r="L57" s="4">
@@ -3254,26 +4129,26 @@
         <v>20</v>
       </c>
       <c r="C58" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130007</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130006</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130018</v>
       </c>
       <c r="E58" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>26.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H58" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>350000</v>
       </c>
       <c r="I58" s="4">
@@ -3283,7 +4158,7 @@
         <v>30</v>
       </c>
       <c r="K58" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1435000</v>
       </c>
       <c r="L58" s="4">
@@ -3299,26 +4174,26 @@
         <v>82</v>
       </c>
       <c r="C59" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130010</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130003</v>
       </c>
       <c r="D59" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130006</v>
       </c>
       <c r="E59" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>12.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>26.6</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H59" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>150000</v>
       </c>
       <c r="I59" s="4">
@@ -3328,7 +4203,7 @@
         <v>50</v>
       </c>
       <c r="K59" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>615000</v>
       </c>
       <c r="L59" s="4">
@@ -3344,26 +4219,26 @@
         <v>83</v>
       </c>
       <c r="C60" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130005</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130010</v>
       </c>
       <c r="D60" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130008</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130011</v>
       </c>
       <c r="E60" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>10.4</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6.8</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H60" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>75000</v>
       </c>
       <c r="I60" s="4">
@@ -3373,7 +4248,7 @@
         <v>90</v>
       </c>
       <c r="K60" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>307500</v>
       </c>
       <c r="L60" s="4">
@@ -3389,26 +4264,26 @@
         <v>84</v>
       </c>
       <c r="C61" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130006</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130005</v>
       </c>
       <c r="D61" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130009</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130001</v>
       </c>
       <c r="E61" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>15.7</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>26.4</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H61" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>300000</v>
       </c>
       <c r="I61" s="4">
@@ -3418,7 +4293,7 @@
         <v>20</v>
       </c>
       <c r="K61" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1230000</v>
       </c>
       <c r="L61" s="4">
@@ -3434,26 +4309,26 @@
         <v>85</v>
       </c>
       <c r="C62" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>LSP202312130009</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>LSP202312130008</v>
       </c>
       <c r="D62" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>NCC202312130003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>NCC202312130015</v>
       </c>
       <c r="E62" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>11.6</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>17.899999999999999</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H62" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100000</v>
       </c>
       <c r="I62" s="4">
@@ -3463,7 +4338,7 @@
         <v>35</v>
       </c>
       <c r="K62" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>410000</v>
       </c>
       <c r="L62" s="4">

</xml_diff>

<commit_message>
fix insert db, insert ex
</commit_message>
<xml_diff>
--- a/src/main/resources/DataImports/SanPham.xlsx
+++ b/src/main/resources/DataImports/SanPham.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PTUD_APP\Manager_QuanLyHieuSach\src\main\resources\DataImports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C983C-8382-4EE8-B826-58B0C8278A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0F0164-83D6-4BE9-9A79-9ABBC8636271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4A98E7E-91B4-4117-82EF-535CA966D02F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B4A98E7E-91B4-4117-82EF-535CA966D02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính3" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="198">
   <si>
     <t>idSanPham</t>
   </si>
@@ -404,94 +404,238 @@
     <t>Công ty Đồ Chơi Giáo Dục Thông Minh</t>
   </si>
   <si>
-    <t>890 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>891 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>892 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>893 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>894 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>895 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
     <t>896 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
   </si>
   <si>
     <t>897 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
   </si>
   <si>
-    <t>898 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>899 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>900 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>901 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>902 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>903 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>904 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>905 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>906 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>907 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>908 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>909 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>910 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>911 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>912 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>913 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>914 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>915 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>916 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
-    <t>917 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
-  </si>
-  <si>
     <t>918 Đường Phan Chu Trinh, Quận Bình Thạnh</t>
   </si>
   <si>
-    <t>hoang</t>
+    <t>Sổ tay và sổ ghi chú</t>
+  </si>
+  <si>
+    <t>Trò chơi chiến lược và bảng</t>
+  </si>
+  <si>
+    <t>Vật phẩm văn phòng hiện đại</t>
+  </si>
+  <si>
+    <t>Phim và bộ sưu tập hình ảnh</t>
+  </si>
+  <si>
+    <t>Sổ tay thông minh</t>
+  </si>
+  <si>
+    <t>Đồ chơi sáng tạo</t>
+  </si>
+  <si>
+    <t>Trò chơi học thuật và giáo dục</t>
+  </si>
+  <si>
+    <t>Đồ chơi giáo dục STEM</t>
+  </si>
+  <si>
+    <t>Đồ chơi sáng tạo cho trẻ em</t>
+  </si>
+  <si>
+    <t>Công ty Sách Truyện Thiếu Nhi</t>
+  </si>
+  <si>
+    <t>Công ty Văn Phòng Phẩm Sáng Tạo</t>
+  </si>
+  <si>
+    <t>Công ty Quà Tặng Sách Nghệ Thuật</t>
+  </si>
+  <si>
+    <t>Công ty Văn Phòng Phẩm Chất Lượng</t>
+  </si>
+  <si>
+    <t>Công ty Đồ Dùng Học Tập Tiện Lợi</t>
+  </si>
+  <si>
+    <t>Công ty Sách Ngoại Văn Pháp Văn</t>
+  </si>
+  <si>
+    <t>Công ty Quà Tặng Văn Hóa Nhật</t>
+  </si>
+  <si>
+    <t>Công ty Sách Khoa Học Phổ Thông</t>
+  </si>
+  <si>
+    <t>Công ty Đồ Chơi Giáo Dục Vui Nhộn</t>
+  </si>
+  <si>
+    <t>Công ty Sách Truyện Thiếu Niên</t>
+  </si>
+  <si>
+    <t>Công ty Văn Phòng Phẩm Đa Dạng</t>
+  </si>
+  <si>
+    <t>123 Đường Nguyễn Văn Linh, Quận 1, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>456 Đường Lê Lai, Quận 3, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>789 Đường Lê Thị Riêng, Quận 5, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>234 Đường Bà Triệu, Quận 7, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>567 Đường Đống Đa, Quận 10, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>321 Đường Hoàng Sa, Q. Phú Nhuận, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>654 Đường Cách Mạng Tháng 8</t>
+  </si>
+  <si>
+    <t>111 Đường Trần Hưng Đạo</t>
+  </si>
+  <si>
+    <t>22 Đường Trần Hưng Đạo, Quận 1, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>12 Đường Nguyễn Thị Minh Khai, Quận 1, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>34 Đường Lý Tự Trọng, Quận 3, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>90 Đường Cao Thắng, Quận 10, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>78 Đường Nguyễn Đình Chiểu, Quận 7, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>33 Đường Phan Đăng Lưu, Quận Phú Nhuận, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>55 Đường Nguyễn Văn Cừ, Quận 11, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>77 Đường Lê Văn Sỹ, Quận Tân Bình, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>99 Đường Nguyễn Thị Thập, Quận 7, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>44 Đường Lê Thánh Tôn, Quận 3, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>66 Đường Trần Phú, Quận 5, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>88 Đường Nguyễn Thái Học, Quận 7, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>111 Đường Lý Thường Kiệt, Quận 10, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>222 Đường Nguyễn Văn Cừ, Quận Bình Thạnh, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>333 Đường Nguyễn Kiệm, Quận Phú Nhuận, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>444 Đường Lê Đại Hành, Quận 11, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>555 Đường Bạch Đằng, Quận Tân Bình, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>666 Đường Nguyễn Hữu Thọ, Quận 7, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>0912345679</t>
+  </si>
+  <si>
+    <t>0912345680</t>
+  </si>
+  <si>
+    <t>0912345681</t>
+  </si>
+  <si>
+    <t>0912345682</t>
+  </si>
+  <si>
+    <t>0912345683</t>
+  </si>
+  <si>
+    <t>0912345684</t>
+  </si>
+  <si>
+    <t>0912345685</t>
+  </si>
+  <si>
+    <t>0912345686</t>
+  </si>
+  <si>
+    <t>0912345687</t>
+  </si>
+  <si>
+    <t>0912345688</t>
+  </si>
+  <si>
+    <t>0912345689</t>
+  </si>
+  <si>
+    <t>0912345690</t>
+  </si>
+  <si>
+    <t>0912345691</t>
+  </si>
+  <si>
+    <t>0912345692</t>
+  </si>
+  <si>
+    <t>0912345693</t>
+  </si>
+  <si>
+    <t>0912345694</t>
+  </si>
+  <si>
+    <t>0912345695</t>
+  </si>
+  <si>
+    <t>0912345696</t>
+  </si>
+  <si>
+    <t>0912345697</t>
+  </si>
+  <si>
+    <t>0912345698</t>
+  </si>
+  <si>
+    <t>0912345699</t>
+  </si>
+  <si>
+    <t>0912345700</t>
+  </si>
+  <si>
+    <t>0912345701</t>
+  </si>
+  <si>
+    <t>0912345702</t>
+  </si>
+  <si>
+    <t>0912345703</t>
+  </si>
+  <si>
+    <t>0912345704</t>
+  </si>
+  <si>
+    <t>0912345705</t>
+  </si>
+  <si>
+    <t>0912345706</t>
   </si>
 </sst>
 </file>
@@ -526,12 +670,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -552,8 +711,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -868,18 +1027,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E5C01E-DF7C-47B1-A3AD-5B43A2BED607}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D30"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" customWidth="1"/>
+    <col min="5" max="6" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,122 +1058,122 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
-        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130019</v>
+        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; "0001"</f>
+        <v>NCC202312130001</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f t="shared" ref="A3:D23" ca="1" si="0">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130011</v>
+        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A2), "0000")</f>
+        <v>NCC202312130002</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130014</v>
+        <f t="shared" ref="A4:A30" ca="1" si="0">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A3), "0000")</f>
+        <v>NCC202312130003</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130008</v>
+        <v>NCC202312130004</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130007</v>
+        <v>NCC202312130005</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130002</v>
+        <v>NCC202312130006</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130021</v>
+        <v>NCC202312130007</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130006</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,314 +1185,313 @@
         <v>110</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130017</v>
+        <v>NCC202312130010</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130007</v>
+        <v>NCC202312130011</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130023</v>
+        <v>NCC202312130012</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130011</v>
+        <v>NCC202312130013</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130020</v>
+        <v>NCC202312130014</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130013</v>
+        <v>NCC202312130015</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130021</v>
+        <v>NCC202312130016</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130013</v>
+        <v>NCC202312130017</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130009</v>
+        <v>NCC202312130018</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130011</v>
+        <v>NCC202312130019</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130005</v>
+        <v>NCC202312130020</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130022</v>
+        <v>NCC202312130021</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCC202312130001</v>
+        <v>NCC202312130022</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
-        <f t="shared" ref="A24:A30" ca="1" si="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130014</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130023</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130011</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130024</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130014</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130025</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130026</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130022</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130027</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130001</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130028</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130014</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>NCC202312130029</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D26" xr:uid="{35E5C01E-DF7C-47B1-A3AD-5B43A2BED607}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1343,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8B4145-E7A7-4BF3-B67B-1D4E4FEF9CC8}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1363,56 +1522,56 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130007</v>
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; "0001"</f>
+        <v>LSP202312130001</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A20" ca="1" si="0">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130007</v>
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A2), "0000")</f>
+        <v>LSP202312130002</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130004</v>
+        <f t="shared" ref="A4:A20" ca="1" si="0">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(ROW(A3), "0000")</f>
+        <v>LSP202312130003</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1421,40 +1580,40 @@
         <v>LSP202312130007</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130009</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130011</v>
       </c>
       <c r="B12" t="s">
         <v>97</v>
@@ -1463,73 +1622,73 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130012</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130013</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130014</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130015</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130016</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130017</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130018</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130019</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1701,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1613,12 +1772,12 @@
         <v>LSP202312130003</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130001</v>
+        <f ca="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 29), "0000")</f>
+        <v>NCC202312130025</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>25.5</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1655,22 +1814,22 @@
       </c>
       <c r="C3" s="3" t="str">
         <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130010</v>
+        <v>LSP202312130007</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D62" ca="1" si="1">"NCC" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(1, 23), "0000")</f>
-        <v>NCC202312130007</v>
+        <v>NCC202312130017</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>15.5</v>
+        <v>5.7</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ref="G3:G62" ca="1" si="2">IF(RAND() &lt;= 0.8, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H62" si="3">I3*0.5</f>
@@ -1699,16 +1858,16 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130004</v>
+        <f ca="1">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 19), "0000")</f>
+        <v>LSP202312130011</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130023</v>
+        <v>NCC202312130009</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E62" ca="1" si="5">ROUND(RAND()*(30-5)+5, 1)</f>
-        <v>14.3</v>
+        <v>20.5</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -1745,15 +1904,15 @@
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" ref="C5:C62" ca="1" si="6">"LSP" &amp; TEXT(TODAY(), "yyyyMMdd") &amp; TEXT(RANDBETWEEN(2, 10), "0000")</f>
-        <v>LSP202312130006</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>27.1</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -1790,15 +1949,15 @@
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130016</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>8.8000000000000007</v>
+        <v>14.6</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
@@ -1835,15 +1994,15 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130007</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130017</v>
+        <v>NCC202312130014</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>12.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>23</v>
@@ -1880,15 +2039,15 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130009</v>
+        <v>NCC202312130006</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>11.2</v>
+        <v>24.9</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>25</v>
@@ -1925,22 +2084,22 @@
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130010</v>
+        <v>NCC202312130020</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>7.7</v>
+        <v>6.4</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="3"/>
@@ -1970,15 +2129,15 @@
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130022</v>
+        <v>NCC202312130011</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>23.1</v>
+        <v>27.5</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -2015,22 +2174,22 @@
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130020</v>
+        <v>NCC202312130019</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>21.1</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="3"/>
@@ -2060,15 +2219,15 @@
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130002</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.2</v>
+        <v>15.7</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
@@ -2105,15 +2264,15 @@
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130021</v>
+        <v>NCC202312130012</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>15.5</v>
+        <v>7.3</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
@@ -2150,15 +2309,15 @@
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130023</v>
+        <v>NCC202312130001</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>22.8</v>
+        <v>15.5</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -2195,22 +2354,22 @@
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130013</v>
+        <v>NCC202312130003</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>17.2</v>
+        <v>15.1</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="3"/>
@@ -2240,15 +2399,15 @@
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130021</v>
+        <v>NCC202312130012</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.8</v>
+        <v>15.6</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
@@ -2285,22 +2444,22 @@
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130001</v>
+        <v>NCC202312130020</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>10.9</v>
+        <v>23.3</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="3"/>
@@ -2330,15 +2489,15 @@
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130005</v>
+        <v>NCC202312130014</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>29.2</v>
+        <v>26.6</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
@@ -2375,7 +2534,7 @@
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2383,14 +2542,14 @@
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>10.5</v>
+        <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="3"/>
@@ -2420,22 +2579,22 @@
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130007</v>
+        <v>NCC202312130015</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>13.5</v>
+        <v>24.5</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="3"/>
@@ -2465,15 +2624,15 @@
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130012</v>
+        <v>NCC202312130007</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>20.2</v>
+        <v>24.4</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>25</v>
@@ -2510,15 +2669,15 @@
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130001</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.1</v>
+        <v>25.8</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>43</v>
@@ -2555,22 +2714,22 @@
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>9.9</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="3"/>
@@ -2600,15 +2759,15 @@
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130003</v>
+        <v>NCC202312130019</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.9</v>
+        <v>16.2</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>21</v>
@@ -2645,22 +2804,22 @@
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130019</v>
+        <v>NCC202312130013</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>19.8</v>
+        <v>10.8</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="3"/>
@@ -2690,15 +2849,15 @@
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130023</v>
+        <v>NCC202312130018</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>18.899999999999999</v>
+        <v>26.5</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>19</v>
@@ -2735,15 +2894,15 @@
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130009</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130004</v>
+        <v>NCC202312130017</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>20.9</v>
+        <v>29.3</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
@@ -2780,15 +2939,15 @@
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130017</v>
+        <v>NCC202312130015</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.3</v>
+        <v>5.5</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>51</v>
@@ -2825,15 +2984,15 @@
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130021</v>
+        <v>NCC202312130018</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>11.4</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>21</v>
@@ -2870,15 +3029,15 @@
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130014</v>
+        <v>NCC202312130016</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>17.3</v>
+        <v>10.8</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>54</v>
@@ -2915,22 +3074,22 @@
       </c>
       <c r="C31" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130004</v>
+        <v>NCC202312130018</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>21.6</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="3"/>
@@ -2960,22 +3119,22 @@
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130022</v>
+        <v>NCC202312130009</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>24.2</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="3"/>
@@ -3005,7 +3164,7 @@
       </c>
       <c r="C33" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3013,14 +3172,14 @@
       </c>
       <c r="E33" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>11.5</v>
+        <v>26.1</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="3"/>
@@ -3050,22 +3209,22 @@
       </c>
       <c r="C34" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130015</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>6.9</v>
+        <v>25.3</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="3"/>
@@ -3095,15 +3254,15 @@
       </c>
       <c r="C35" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130004</v>
+        <v>NCC202312130009</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>23.9</v>
+        <v>28.6</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>25</v>
@@ -3140,15 +3299,15 @@
       </c>
       <c r="C36" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130009</v>
+        <v>LSP202312130007</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130012</v>
+        <v>NCC202312130003</v>
       </c>
       <c r="E36" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>7.5</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>23</v>
@@ -3189,11 +3348,11 @@
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130012</v>
+        <v>NCC202312130007</v>
       </c>
       <c r="E37" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>7.7</v>
+        <v>22.2</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
@@ -3230,15 +3389,15 @@
       </c>
       <c r="C38" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130009</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130014</v>
+        <v>NCC202312130011</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>15.6</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
@@ -3275,15 +3434,15 @@
       </c>
       <c r="C39" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130015</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>19.600000000000001</v>
+        <v>29</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>31</v>
@@ -3320,22 +3479,22 @@
       </c>
       <c r="C40" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130007</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130004</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>5.6</v>
+        <v>25.3</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G40" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4">
         <f t="shared" si="3"/>
@@ -3365,22 +3524,22 @@
       </c>
       <c r="C41" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>6.1</v>
+        <v>27.6</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" si="3"/>
@@ -3410,7 +3569,7 @@
       </c>
       <c r="C42" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3418,14 +3577,14 @@
       </c>
       <c r="E42" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>19.7</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="3"/>
@@ -3455,15 +3614,15 @@
       </c>
       <c r="C43" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130019</v>
+        <v>NCC202312130020</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>13.1</v>
+        <v>11.8</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>21</v>
@@ -3504,11 +3663,11 @@
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130016</v>
+        <v>NCC202312130022</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>18.7</v>
+        <v>21.1</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>25</v>
@@ -3549,11 +3708,11 @@
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130010</v>
+        <v>NCC202312130013</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>27.8</v>
+        <v>14.3</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>43</v>
@@ -3590,22 +3749,22 @@
       </c>
       <c r="C46" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130014</v>
+        <v>NCC202312130007</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>26.6</v>
+        <v>27.4</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G46" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="3"/>
@@ -3635,15 +3794,15 @@
       </c>
       <c r="C47" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130002</v>
+        <v>NCC202312130010</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>27.2</v>
+        <v>29.8</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>54</v>
@@ -3680,15 +3839,15 @@
       </c>
       <c r="C48" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130019</v>
+        <v>NCC202312130001</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>11.8</v>
+        <v>27.3</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>13</v>
@@ -3725,22 +3884,22 @@
       </c>
       <c r="C49" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130010</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130021</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>13.7</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="4">
         <f t="shared" si="3"/>
@@ -3774,18 +3933,18 @@
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130011</v>
+        <v>NCC202312130010</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>5.8</v>
+        <v>5.2</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="4">
         <f t="shared" si="3"/>
@@ -3815,22 +3974,22 @@
       </c>
       <c r="C51" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130006</v>
+        <v>LSP202312130009</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>25.9</v>
+        <v>28.3</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="4">
         <f t="shared" si="3"/>
@@ -3860,15 +4019,15 @@
       </c>
       <c r="C52" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130007</v>
+        <v>LSP202312130008</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130011</v>
+        <v>NCC202312130013</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>11.3</v>
+        <v>15.3</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
@@ -3905,15 +4064,15 @@
       </c>
       <c r="C53" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130007</v>
+        <v>NCC202312130002</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>21.9</v>
+        <v>12.9</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
@@ -3950,15 +4109,15 @@
       </c>
       <c r="C54" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130006</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130012</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>22.5</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>21</v>
@@ -3995,15 +4154,15 @@
       </c>
       <c r="C55" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130007</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130020</v>
+        <v>NCC202312130015</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>29.1</v>
+        <v>8</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>13</v>
@@ -4040,15 +4199,15 @@
       </c>
       <c r="C56" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130004</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130006</v>
+        <v>NCC202312130022</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>23</v>
+        <v>10.9</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
@@ -4085,15 +4244,15 @@
       </c>
       <c r="C57" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130002</v>
+        <v>LSP202312130005</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130013</v>
+        <v>NCC202312130014</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>6.7</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>81</v>
@@ -4134,11 +4293,11 @@
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130018</v>
+        <v>NCC202312130010</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>15.7</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>21</v>
@@ -4175,22 +4334,22 @@
       </c>
       <c r="C59" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130003</v>
+        <v>LSP202312130002</v>
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130006</v>
+        <v>NCC202312130010</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>26.6</v>
+        <v>23.5</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="3"/>
@@ -4220,15 +4379,15 @@
       </c>
       <c r="C60" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130010</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130011</v>
+        <v>NCC202312130008</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>6.8</v>
+        <v>13.1</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>21</v>
@@ -4265,22 +4424,22 @@
       </c>
       <c r="C61" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130005</v>
+        <v>LSP202312130004</v>
       </c>
       <c r="D61" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130001</v>
+        <v>NCC202312130012</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>26.4</v>
+        <v>27.6</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G61" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="3"/>
@@ -4310,15 +4469,15 @@
       </c>
       <c r="C62" s="3" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSP202312130008</v>
+        <v>LSP202312130003</v>
       </c>
       <c r="D62" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NCC202312130015</v>
+        <v>NCC202312130004</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>17.899999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>

</xml_diff>